<commit_message>
trying to get concurrency running
</commit_message>
<xml_diff>
--- a/MATLAB/newCCM/Crystal Database New.xlsx
+++ b/MATLAB/newCCM/Crystal Database New.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Matt\Documents\GitHub\DNA-NP-Prediction\MATLAB\newCCM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="345">
   <si>
     <t>Crystal Type</t>
   </si>
@@ -1045,6 +1050,15 @@
   </si>
   <si>
     <t>Distance</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>hmmm</t>
+  </si>
+  <si>
+    <t>Fm3m</t>
   </si>
 </sst>
 </file>
@@ -1425,7 +1439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1435,9 +1449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A108" sqref="A108"/>
+      <selection pane="topRight" activeCell="V105" sqref="V105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8583,23 +8597,74 @@
       </c>
     </row>
     <row r="104" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F104" s="14"/>
-      <c r="G104" s="14"/>
-      <c r="H104" s="14"/>
-      <c r="I104" s="14"/>
-      <c r="J104" s="14"/>
-      <c r="K104" s="14"/>
-      <c r="L104" s="14"/>
-      <c r="M104" s="14"/>
-      <c r="N104" s="14"/>
-      <c r="O104" s="14"/>
-      <c r="P104" s="14"/>
-      <c r="Q104" s="14"/>
-      <c r="R104" s="14"/>
-      <c r="S104" s="14"/>
-      <c r="T104" s="14"/>
-      <c r="U104" s="14"/>
-      <c r="V104" s="14"/>
+      <c r="A104" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104" s="14">
+        <v>1</v>
+      </c>
+      <c r="G104" s="14">
+        <v>1</v>
+      </c>
+      <c r="H104" s="14">
+        <v>0</v>
+      </c>
+      <c r="I104" s="14">
+        <v>6</v>
+      </c>
+      <c r="J104" s="14">
+        <v>6</v>
+      </c>
+      <c r="K104" s="14">
+        <v>0</v>
+      </c>
+      <c r="L104" s="1">
+        <v>1</v>
+      </c>
+      <c r="M104" s="14">
+        <v>12</v>
+      </c>
+      <c r="N104" s="14">
+        <v>0</v>
+      </c>
+      <c r="O104" s="14">
+        <v>0</v>
+      </c>
+      <c r="P104" s="14">
+        <v>12</v>
+      </c>
+      <c r="Q104" s="1">
+        <f>SQRT(2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="R104" s="14">
+        <v>0</v>
+      </c>
+      <c r="S104" s="14">
+        <v>6</v>
+      </c>
+      <c r="T104" s="14">
+        <v>6</v>
+      </c>
+      <c r="U104" s="14">
+        <v>0</v>
+      </c>
+      <c r="V104" s="14">
+        <f>SQRT(3)</f>
+        <v>1.7320508075688772</v>
+      </c>
     </row>
     <row r="105" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F105" s="14"/>
@@ -9206,6 +9271,6 @@
     <mergeCell ref="R2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>